<commit_message>
updated results with bwa and bowtie
git-svn-id: file://localhost/tmp/svn2git/svn@5509 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/chipseq_test.xlsx
+++ b/papers/data-intensive-bio/results/chipseq_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t>Ref-Genome</t>
   </si>
@@ -78,15 +78,6 @@
     <t>TIME for MACS(Sec)</t>
   </si>
   <si>
-    <t>Control Data Size</t>
-  </si>
-  <si>
-    <t>6.3 Gb</t>
-  </si>
-  <si>
-    <t>5.5 GB</t>
-  </si>
-  <si>
     <t xml:space="preserve">100MB </t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>Temp Space Required per file(GB)</t>
   </si>
   <si>
-    <t>11.8 Gb</t>
-  </si>
-  <si>
     <t>Total Space required for all files(GB)</t>
   </si>
   <si>
@@ -127,13 +115,49 @@
   </si>
   <si>
     <t>App Temp for  mapping</t>
+  </si>
+  <si>
+    <t>BWA</t>
+  </si>
+  <si>
+    <t>BOWTIE</t>
+  </si>
+  <si>
+    <t>400MB</t>
+  </si>
+  <si>
+    <t>114 MB</t>
+  </si>
+  <si>
+    <t>122 MB</t>
+  </si>
+  <si>
+    <t>245MB</t>
+  </si>
+  <si>
+    <t>480 MB</t>
+  </si>
+  <si>
+    <t>449 MB</t>
+  </si>
+  <si>
+    <t>229 MB</t>
+  </si>
+  <si>
+    <t>23MB</t>
+  </si>
+  <si>
+    <t>12Mb</t>
+  </si>
+  <si>
+    <t>5.7 MB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -192,7 +223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -217,14 +248,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="40">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -236,6 +284,14 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -248,6 +304,14 @@
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:L20"/>
+  <dimension ref="A4:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -596,12 +660,12 @@
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12">
+    <row r="4" spans="1:12">
       <c r="J4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:12" s="1" customFormat="1" ht="58" thickBot="1">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="58" thickBot="1">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="16" thickTop="1">
+    <row r="6" spans="1:12" ht="16" thickTop="1">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -641,7 +705,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -665,7 +729,7 @@
         <v>136.41</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="1:12">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -673,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -697,112 +761,270 @@
         <v>181.7</v>
       </c>
     </row>
-    <row r="13" spans="2:12" s="1" customFormat="1" ht="39" thickBot="1">
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>182.96</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>307.47000000000003</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>542.65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>167.18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15">
+        <v>277.58999999999997</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="2">
+        <v>507.61</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="1" customFormat="1" ht="77" thickBot="1">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="16" thickTop="1">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" ht="16" thickTop="1">
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12">
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" s="1" customFormat="1" ht="77" thickBot="1">
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="16" thickTop="1">
-      <c r="B18" t="s">
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="C18">
-        <v>40</v>
-      </c>
-      <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18">
+      <c r="F20">
         <f>16*45/1000</f>
         <v>0.72</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <f>118 *0.72</f>
         <v>84.96</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19">
+    <row r="21" spans="2:7">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
         <v>40</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19">
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21">
         <f>16*89/1000</f>
         <v>1.4239999999999999</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <f>59*1.424</f>
         <v>84.015999999999991</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20">
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
         <v>40</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20">
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22">
         <f>16*175/1000</f>
         <v>2.8</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <f>30*2.8</f>
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
updated results with bowtie
git-svn-id: file://localhost/tmp/svn2git/svn@5529 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/chipseq_test.xlsx
+++ b/papers/data-intensive-bio/results/chipseq_test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Ref-Genome</t>
   </si>
@@ -142,6 +142,30 @@
   </si>
   <si>
     <t>229 MB</t>
+  </si>
+  <si>
+    <t>129M</t>
+  </si>
+  <si>
+    <t>121M</t>
+  </si>
+  <si>
+    <t>257MB</t>
+  </si>
+  <si>
+    <t>241MB</t>
+  </si>
+  <si>
+    <t>128M</t>
+  </si>
+  <si>
+    <t>163MB</t>
+  </si>
+  <si>
+    <t>504MB</t>
+  </si>
+  <si>
+    <t>472MB</t>
   </si>
 </sst>
 </file>
@@ -214,9 +238,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="40">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -263,7 +289,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="40">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -283,6 +309,7 @@
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -303,6 +330,7 @@
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -635,13 +663,13 @@
   <dimension ref="A4:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:I16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
@@ -779,6 +807,9 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
@@ -802,6 +833,9 @@
       <c r="D11" t="s">
         <v>21</v>
       </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
       <c r="F11" t="s">
         <v>32</v>
       </c>
@@ -825,6 +859,9 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
       <c r="F12" t="s">
         <v>32</v>
       </c>
@@ -848,8 +885,20 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
       <c r="F14" t="s">
         <v>33</v>
+      </c>
+      <c r="G14">
+        <v>156.96</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -862,8 +911,20 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
       <c r="F15" t="s">
         <v>33</v>
+      </c>
+      <c r="G15">
+        <v>277.3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -877,13 +938,21 @@
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F16" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="G16" s="2">
+        <v>497.73</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>

</xml_diff>

<commit_message>
updated results with postprocess
git-svn-id: file://localhost/tmp/svn2git/svn@5531 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/chipseq_test.xlsx
+++ b/papers/data-intensive-bio/results/chipseq_test.xlsx
@@ -238,9 +238,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -289,7 +299,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -310,6 +320,11 @@
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -331,6 +346,11 @@
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:L22"/>
+  <dimension ref="A4:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -742,10 +762,10 @@
         <v>13</v>
       </c>
       <c r="J6">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="L6">
-        <v>136.41</v>
+        <v>152.78</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -774,10 +794,10 @@
         <v>16</v>
       </c>
       <c r="J7">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="L7">
-        <v>181.7</v>
+        <v>217.66</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -822,6 +842,12 @@
       <c r="I10" t="s">
         <v>36</v>
       </c>
+      <c r="J10">
+        <v>33</v>
+      </c>
+      <c r="L10">
+        <v>142.34</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
@@ -848,6 +874,12 @@
       <c r="I11" t="s">
         <v>37</v>
       </c>
+      <c r="J11">
+        <v>52</v>
+      </c>
+      <c r="L11">
+        <v>202.22</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
@@ -900,6 +932,12 @@
       <c r="I14" t="s">
         <v>41</v>
       </c>
+      <c r="J14">
+        <v>30</v>
+      </c>
+      <c r="L14">
+        <v>137.33000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
@@ -925,6 +963,12 @@
       </c>
       <c r="I15" t="s">
         <v>43</v>
+      </c>
+      <c r="J15">
+        <v>60</v>
+      </c>
+      <c r="L15">
+        <v>177.45</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1046,6 +1090,22 @@
       <c r="G22">
         <f>30*2.8</f>
         <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="10:12">
+      <c r="J41">
+        <v>68</v>
+      </c>
+      <c r="L41">
+        <v>181.7</v>
+      </c>
+    </row>
+    <row r="42" spans="10:12">
+      <c r="J42">
+        <v>35</v>
+      </c>
+      <c r="L42">
+        <v>136.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving new chipseq figure
git-svn-id: file://localhost/tmp/svn2git/svn@5634 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/chipseq_test.xlsx
+++ b/papers/data-intensive-bio/results/chipseq_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17200" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26140" windowHeight="16340" tabRatio="320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Ref-Genome</t>
   </si>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t>Ref. Genome index file size</t>
+  </si>
+  <si>
+    <t>118 files</t>
+  </si>
+  <si>
+    <t>118 file</t>
+  </si>
+  <si>
+    <t>118files</t>
+  </si>
+  <si>
+    <t>bowtie</t>
+  </si>
+  <si>
+    <t>bwa</t>
+  </si>
+  <si>
+    <t>bfast</t>
   </si>
 </sst>
 </file>
@@ -238,9 +256,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="58">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,7 +327,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="58">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -334,6 +356,8 @@
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -363,6 +387,8 @@
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,11 +471,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="774096376"/>
-        <c:axId val="774099352"/>
+        <c:axId val="671867704"/>
+        <c:axId val="671663320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="774096376"/>
+        <c:axId val="671867704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="774099352"/>
+        <c:crossAx val="671663320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -476,7 +502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="774099352"/>
+        <c:axId val="671663320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="774096376"/>
+        <c:crossAx val="671867704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -883,15 +909,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:L42"/>
+  <dimension ref="A4:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
@@ -1335,6 +1362,45 @@
         <v>136.41</v>
       </c>
     </row>
+    <row r="68" spans="6:6">
+      <c r="F68">
+        <f>2119/60</f>
+        <v>35.31666666666667</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7">
+      <c r="C83" t="s">
+        <v>50</v>
+      </c>
+      <c r="F83" t="s">
+        <v>52</v>
+      </c>
+      <c r="G83">
+        <v>265.43633389500002</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7">
+      <c r="C84" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84" t="s">
+        <v>53</v>
+      </c>
+      <c r="G84">
+        <v>326.09100000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7">
+      <c r="C85" t="s">
+        <v>51</v>
+      </c>
+      <c r="F85" t="s">
+        <v>54</v>
+      </c>
+      <c r="G85">
+        <v>2245.7800000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated figure scaling in tex
git-svn-id: file://localhost/tmp/svn2git/svn@5702 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/chipseq_test.xlsx
+++ b/papers/data-intensive-bio/results/chipseq_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26140" windowHeight="16340" tabRatio="320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Ref-Genome</t>
   </si>
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,6 +229,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,12 +327,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -471,11 +479,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="671867704"/>
-        <c:axId val="671663320"/>
+        <c:axId val="537535960"/>
+        <c:axId val="537538936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="671867704"/>
+        <c:axId val="537535960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,17 +492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1500"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="671663320"/>
+        <c:crossAx val="537538936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -502,7 +500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="671663320"/>
+        <c:axId val="537538936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +516,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1500"/>
-                  <a:t>Time </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1500" baseline="0"/>
-                  <a:t> for Mapping(Sec)</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time  for Mapping(Sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -535,7 +529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="671867704"/>
+        <c:crossAx val="537535960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -544,6 +538,168 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1500"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$98:$C$100</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>BFAST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BWA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BOWTIE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$98:$D$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3402.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2545.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="537599560"/>
+        <c:axId val="537602504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="537599560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="537602504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="537602504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of Predicted Peaks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="537599560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1500"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -579,6 +735,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -909,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:L85"/>
+  <dimension ref="A4:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1401,6 +1587,30 @@
         <v>2245.7800000000002</v>
       </c>
     </row>
+    <row r="98" spans="3:4" ht="18">
+      <c r="C98" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" ht="18">
+      <c r="C99" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D99">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" ht="18">
+      <c r="C100" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100">
+        <v>2545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>